<commit_message>
First part of tests
</commit_message>
<xml_diff>
--- a/DaneDoTestów.xlsx
+++ b/DaneDoTestów.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
@@ -670,7 +670,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,18 +705,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -858,10 +846,10 @@
   </sheetPr>
   <dimension ref="A1:AX43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AL1" activeCellId="0" sqref="AL1"/>
-      <selection pane="bottomLeft" activeCell="AX42" activeCellId="0" sqref="AX42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="AK1" activeCellId="0" sqref="AK1"/>
+      <selection pane="bottomLeft" activeCell="AX52" activeCellId="0" sqref="AX52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3761,7 +3749,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -3848,32 +3836,32 @@
         <v>0</v>
       </c>
       <c r="AA17" s="7" t="n">
-        <f aca="false">IF(M17="TAK",Arkusz3!$B$20*J17,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M17="TAK",Arkusz3!$B$19*J17,0)</f>
+        <v>5</v>
       </c>
       <c r="AB17" s="7" t="n">
-        <f aca="false">IF(N17="TAK",Arkusz3!$B$21*J17,0)</f>
+        <f aca="false">IF(N17="TAK",Arkusz3!$B$19*J17,0)</f>
         <v>0</v>
       </c>
       <c r="AC17" s="7" t="n">
-        <f aca="false">IF(O17="TAK",Arkusz3!$B$22*J17,0)</f>
+        <f aca="false">IF(O17="TAK",Arkusz3!$B$19*J17,0)</f>
         <v>0</v>
       </c>
       <c r="AD17" s="7" t="n">
-        <f aca="false">IF(P17="TAK",Arkusz3!$B$23*J17,0)</f>
+        <f aca="false">IF(P17="TAK",Arkusz3!$B$19*J17,0)</f>
         <v>0</v>
       </c>
       <c r="AE17" s="7" t="n">
-        <f aca="false">IF(Q17="TAK",Arkusz3!$B$24*J17,0)</f>
+        <f aca="false">IF(Q17="TAK",Arkusz3!$B$19*J17,0)</f>
         <v>5</v>
       </c>
       <c r="AF17" s="7" t="n">
-        <f aca="false">IF(R17="TAK",Arkusz3!$B$25*J17,0)</f>
+        <f aca="false">IF(R17="TAK",Arkusz3!$B$19*J17,0)</f>
         <v>0</v>
       </c>
       <c r="AG17" s="7" t="n">
         <f aca="false">SUM(Z17:AF17)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AH17" s="7" t="n">
         <f aca="false">IF(L17="Nie",0,5)</f>
@@ -3909,7 +3897,7 @@
       </c>
       <c r="AP17" s="7" t="n">
         <f aca="false">IF(AI17&gt;5,AA17*0.2*(AI17-5)+AA17,AA17)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ17" s="7" t="n">
         <f aca="false">IF(AJ17&gt;5,AB17*0.2*(AJ17-5)+AB17,AB17)</f>
@@ -3933,17 +3921,17 @@
       </c>
       <c r="AV17" s="7" t="n">
         <f aca="false">SUM(AO17:AU17)+Y17</f>
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="AW17" s="7" t="n">
         <f aca="false">IF(S17="Roczna",AV17*12*0.95,AV17)</f>
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="AX17" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
@@ -4030,32 +4018,32 @@
         <v>0</v>
       </c>
       <c r="AA18" s="7" t="n">
-        <f aca="false">IF(M18="TAK",Arkusz3!$B$20*J18,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M18="TAK",Arkusz3!$B$19*J18,0)</f>
+        <v>10</v>
       </c>
       <c r="AB18" s="7" t="n">
-        <f aca="false">IF(N18="TAK",Arkusz3!$B$21*J18,0)</f>
+        <f aca="false">IF(N18="TAK",Arkusz3!$B$19*J18,0)</f>
         <v>0</v>
       </c>
       <c r="AC18" s="7" t="n">
-        <f aca="false">IF(O18="TAK",Arkusz3!$B$22*J18,0)</f>
-        <v>20</v>
+        <f aca="false">IF(O18="TAK",Arkusz3!$B$19*J18,0)</f>
+        <v>10</v>
       </c>
       <c r="AD18" s="7" t="n">
-        <f aca="false">IF(P18="TAK",Arkusz3!$B$23*J18,0)</f>
+        <f aca="false">IF(P18="TAK",Arkusz3!$B$19*J18,0)</f>
         <v>0</v>
       </c>
       <c r="AE18" s="7" t="n">
-        <f aca="false">IF(Q18="TAK",Arkusz3!$B$24*J18,0)</f>
+        <f aca="false">IF(Q18="TAK",Arkusz3!$B$19*J18,0)</f>
         <v>10</v>
       </c>
       <c r="AF18" s="7" t="n">
-        <f aca="false">IF(R18="TAK",Arkusz3!$B$25*J18,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R18="TAK",Arkusz3!$B$19*J18,0)</f>
+        <v>10</v>
       </c>
       <c r="AG18" s="7" t="n">
         <f aca="false">SUM(Z18:AF18)</f>
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="AH18" s="7" t="n">
         <f aca="false">IF(L18="Nie",0,5)</f>
@@ -4088,7 +4076,7 @@
       </c>
       <c r="AP18" s="7" t="n">
         <f aca="false">IF(AI18&gt;5,AA18*0.2*(AI18-5)+AA18,AA18)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ18" s="7" t="n">
         <f aca="false">IF(AJ18&gt;5,AB18*0.2*(AJ18-5)+AB18,AB18)</f>
@@ -4096,7 +4084,7 @@
       </c>
       <c r="AR18" s="7" t="n">
         <f aca="false">IF(AK18&gt;5,AC18*0.2*(AK18-5)+AC18,AC18)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS18" s="7" t="n">
         <f aca="false">IF(AL18&gt;5,AD18*0.2*(AL18-5)+AD18,AD18)</f>
@@ -4108,21 +4096,21 @@
       </c>
       <c r="AU18" s="7" t="n">
         <f aca="false">IF(AN18&gt;5,AF18*0.2*(AN18-5)+AF18,AF18)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV18" s="7" t="n">
         <f aca="false">SUM(AO18:AU18)+Y18</f>
-        <v>218.5</v>
+        <v>184.5</v>
       </c>
       <c r="AW18" s="7" t="n">
         <f aca="false">IF(S18="Roczna",AV18*12*0.95,AV18)</f>
-        <v>2490.9</v>
+        <v>2103.3</v>
       </c>
       <c r="AX18" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
@@ -4209,32 +4197,32 @@
         <v>0</v>
       </c>
       <c r="AA19" s="7" t="n">
-        <f aca="false">IF(M19="TAK",Arkusz3!$B$20*J19,0)</f>
+        <f aca="false">IF(M19="TAK",Arkusz3!$B$19*J19,0)</f>
         <v>0</v>
       </c>
       <c r="AB19" s="7" t="n">
-        <f aca="false">IF(N19="TAK",Arkusz3!$B$21*J19,0)</f>
+        <f aca="false">IF(N19="TAK",Arkusz3!$B$19*J19,0)</f>
         <v>0</v>
       </c>
       <c r="AC19" s="7" t="n">
-        <f aca="false">IF(O19="TAK",Arkusz3!$B$22*J19,0)</f>
+        <f aca="false">IF(O19="TAK",Arkusz3!$B$19*J19,0)</f>
         <v>0</v>
       </c>
       <c r="AD19" s="7" t="n">
-        <f aca="false">IF(P19="TAK",Arkusz3!$B$23*J19,0)</f>
+        <f aca="false">IF(P19="TAK",Arkusz3!$B$19*J19,0)</f>
         <v>0</v>
       </c>
       <c r="AE19" s="7" t="n">
-        <f aca="false">IF(Q19="TAK",Arkusz3!$B$24*J19,0)</f>
+        <f aca="false">IF(Q19="TAK",Arkusz3!$B$19*J19,0)</f>
         <v>0</v>
       </c>
       <c r="AF19" s="7" t="n">
-        <f aca="false">IF(R19="TAK",Arkusz3!$B$25*J19,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R19="TAK",Arkusz3!$B$19*J19,0)</f>
+        <v>10</v>
       </c>
       <c r="AG19" s="7" t="n">
         <f aca="false">SUM(Z19:AF19)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AH19" s="7" t="n">
         <f aca="false">IF(L19="Nie",0,5)</f>
@@ -4289,21 +4277,21 @@
       </c>
       <c r="AU19" s="7" t="n">
         <f aca="false">IF(AN19&gt;5,AF19*0.2*(AN19-5)+AF19,AF19)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV19" s="7" t="n">
         <f aca="false">SUM(AO19:AU19)+Y19</f>
-        <v>148.5</v>
+        <v>134.5</v>
       </c>
       <c r="AW19" s="7" t="n">
         <f aca="false">IF(S19="Roczna",AV19*12*0.95,AV19)</f>
-        <v>1692.9</v>
+        <v>1533.3</v>
       </c>
       <c r="AX19" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -4390,32 +4378,32 @@
         <v>0</v>
       </c>
       <c r="AA20" s="7" t="n">
-        <f aca="false">IF(M20="TAK",Arkusz3!$B$20*J20,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M20="TAK",Arkusz3!$B$19*J20,0)</f>
+        <v>10</v>
       </c>
       <c r="AB20" s="7" t="n">
-        <f aca="false">IF(N20="TAK",Arkusz3!$B$21*J20,0)</f>
-        <v>16</v>
+        <f aca="false">IF(N20="TAK",Arkusz3!$B$19*J20,0)</f>
+        <v>10</v>
       </c>
       <c r="AC20" s="7" t="n">
-        <f aca="false">IF(O20="TAK",Arkusz3!$B$22*J20,0)</f>
-        <v>20</v>
+        <f aca="false">IF(O20="TAK",Arkusz3!$B$19*J20,0)</f>
+        <v>10</v>
       </c>
       <c r="AD20" s="7" t="n">
-        <f aca="false">IF(P20="TAK",Arkusz3!$B$23*J20,0)</f>
+        <f aca="false">IF(P20="TAK",Arkusz3!$B$19*J20,0)</f>
         <v>0</v>
       </c>
       <c r="AE20" s="7" t="n">
-        <f aca="false">IF(Q20="TAK",Arkusz3!$B$24*J20,0)</f>
+        <f aca="false">IF(Q20="TAK",Arkusz3!$B$19*J20,0)</f>
         <v>0</v>
       </c>
       <c r="AF20" s="7" t="n">
-        <f aca="false">IF(R20="TAK",Arkusz3!$B$25*J20,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R20="TAK",Arkusz3!$B$19*J20,0)</f>
+        <v>10</v>
       </c>
       <c r="AG20" s="7" t="n">
         <f aca="false">SUM(Z20:AF20)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="AH20" s="7" t="n">
         <f aca="false">IF(L20="Nie",0,5)</f>
@@ -4451,15 +4439,15 @@
       </c>
       <c r="AP20" s="7" t="n">
         <f aca="false">IF(AI20&gt;5,AA20*0.2*(AI20-5)+AA20,AA20)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ20" s="7" t="n">
         <f aca="false">IF(AJ20&gt;5,AB20*0.2*(AJ20-5)+AB20,AB20)</f>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AR20" s="7" t="n">
         <f aca="false">IF(AK20&gt;5,AC20*0.2*(AK20-5)+AC20,AC20)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS20" s="7" t="n">
         <f aca="false">IF(AL20&gt;5,AD20*0.2*(AL20-5)+AD20,AD20)</f>
@@ -4471,15 +4459,15 @@
       </c>
       <c r="AU20" s="7" t="n">
         <f aca="false">IF(AN20&gt;5,AF20*0.2*(AN20-5)+AF20,AF20)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV20" s="7" t="n">
         <f aca="false">SUM(AO20:AU20)+Y20</f>
-        <v>244.5</v>
+        <v>204.5</v>
       </c>
       <c r="AW20" s="7" t="n">
         <f aca="false">IF(S20="Roczna",AV20*12*0.95,AV20)</f>
-        <v>244.5</v>
+        <v>204.5</v>
       </c>
       <c r="AX20" s="7" t="s">
         <v>44</v>
@@ -4572,32 +4560,32 @@
         <v>5</v>
       </c>
       <c r="AA21" s="7" t="n">
-        <f aca="false">IF(M21="TAK",Arkusz3!$B$20*J21,0)</f>
+        <f aca="false">IF(M21="TAK",Arkusz3!$B$19*J21,0)</f>
         <v>0</v>
       </c>
       <c r="AB21" s="7" t="n">
-        <f aca="false">IF(N21="TAK",Arkusz3!$B$21*J21,0)</f>
+        <f aca="false">IF(N21="TAK",Arkusz3!$B$19*J21,0)</f>
         <v>0</v>
       </c>
       <c r="AC21" s="7" t="n">
-        <f aca="false">IF(O21="TAK",Arkusz3!$B$22*J21,0)</f>
+        <f aca="false">IF(O21="TAK",Arkusz3!$B$19*J21,0)</f>
         <v>0</v>
       </c>
       <c r="AD21" s="7" t="n">
-        <f aca="false">IF(P21="TAK",Arkusz3!$B$23*J21,0)</f>
+        <f aca="false">IF(P21="TAK",Arkusz3!$B$19*J21,0)</f>
         <v>0</v>
       </c>
       <c r="AE21" s="7" t="n">
-        <f aca="false">IF(Q21="TAK",Arkusz3!$B$24*J21,0)</f>
+        <f aca="false">IF(Q21="TAK",Arkusz3!$B$19*J21,0)</f>
         <v>5</v>
       </c>
       <c r="AF21" s="7" t="n">
-        <f aca="false">IF(R21="TAK",Arkusz3!$B$25*J21,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R21="TAK",Arkusz3!$B$19*J21,0)</f>
+        <v>5</v>
       </c>
       <c r="AG21" s="7" t="n">
         <f aca="false">SUM(Z21:AF21)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AH21" s="7" t="n">
         <f aca="false">IF(L21="Nie",0,5)</f>
@@ -4653,15 +4641,15 @@
       </c>
       <c r="AU21" s="7" t="n">
         <f aca="false">IF(AN21&gt;5,AF21*0.2*(AN21-5)+AF21,AF21)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV21" s="7" t="n">
         <f aca="false">SUM(AO21:AU21)+Y21</f>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="AW21" s="7" t="n">
         <f aca="false">IF(S21="Roczna",AV21*12*0.95,AV21)</f>
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="AX21" s="7" t="s">
         <v>57</v>
@@ -4754,32 +4742,32 @@
         <v>0</v>
       </c>
       <c r="AA22" s="7" t="n">
-        <f aca="false">IF(M22="TAK",Arkusz3!$B$20*J22,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M22="TAK",Arkusz3!$B$19*J22,0)</f>
+        <v>10</v>
       </c>
       <c r="AB22" s="7" t="n">
-        <f aca="false">IF(N22="TAK",Arkusz3!$B$21*J22,0)</f>
-        <v>16</v>
+        <f aca="false">IF(N22="TAK",Arkusz3!$B$19*J22,0)</f>
+        <v>10</v>
       </c>
       <c r="AC22" s="7" t="n">
-        <f aca="false">IF(O22="TAK",Arkusz3!$B$22*J22,0)</f>
+        <f aca="false">IF(O22="TAK",Arkusz3!$B$19*J22,0)</f>
         <v>0</v>
       </c>
       <c r="AD22" s="7" t="n">
-        <f aca="false">IF(P22="TAK",Arkusz3!$B$23*J22,0)</f>
-        <v>24</v>
+        <f aca="false">IF(P22="TAK",Arkusz3!$B$19*J22,0)</f>
+        <v>10</v>
       </c>
       <c r="AE22" s="7" t="n">
-        <f aca="false">IF(Q22="TAK",Arkusz3!$B$24*J22,0)</f>
+        <f aca="false">IF(Q22="TAK",Arkusz3!$B$19*J22,0)</f>
         <v>0</v>
       </c>
       <c r="AF22" s="7" t="n">
-        <f aca="false">IF(R22="TAK",Arkusz3!$B$25*J22,0)</f>
+        <f aca="false">IF(R22="TAK",Arkusz3!$B$19*J22,0)</f>
         <v>0</v>
       </c>
       <c r="AG22" s="7" t="n">
         <f aca="false">SUM(Z22:AF22)</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="AH22" s="7" t="n">
         <f aca="false">IF(L22="Nie",0,5)</f>
@@ -4813,11 +4801,11 @@
       </c>
       <c r="AP22" s="7" t="n">
         <f aca="false">IF(AI22&gt;5,AA22*0.2*(AI22-5)+AA22,AA22)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ22" s="7" t="n">
         <f aca="false">IF(AJ22&gt;5,AB22*0.2*(AJ22-5)+AB22,AB22)</f>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="AR22" s="7" t="n">
         <f aca="false">IF(AK22&gt;5,AC22*0.2*(AK22-5)+AC22,AC22)</f>
@@ -4825,7 +4813,7 @@
       </c>
       <c r="AS22" s="7" t="n">
         <f aca="false">IF(AL22&gt;5,AD22*0.2*(AL22-5)+AD22,AD22)</f>
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="AT22" s="7" t="n">
         <f aca="false">IF(AM22&gt;5,AE22*0.2*(AM22-5)+AE22,AE22)</f>
@@ -4837,11 +4825,11 @@
       </c>
       <c r="AV22" s="7" t="n">
         <f aca="false">SUM(AO22:AU22)+Y22</f>
-        <v>204.5</v>
+        <v>154.5</v>
       </c>
       <c r="AW22" s="7" t="n">
         <f aca="false">IF(S22="Roczna",AV22*12*0.95,AV22)</f>
-        <v>204.5</v>
+        <v>154.5</v>
       </c>
       <c r="AX22" s="7" t="s">
         <v>44</v>
@@ -4934,32 +4922,32 @@
         <v>0</v>
       </c>
       <c r="AA23" s="7" t="n">
-        <f aca="false">IF(M23="TAK",Arkusz3!$B$20*J23,0)</f>
+        <f aca="false">IF(M23="TAK",Arkusz3!$B$19*J23,0)</f>
         <v>0</v>
       </c>
       <c r="AB23" s="7" t="n">
-        <f aca="false">IF(N23="TAK",Arkusz3!$B$21*J23,0)</f>
+        <f aca="false">IF(N23="TAK",Arkusz3!$B$19*J23,0)</f>
         <v>0</v>
       </c>
       <c r="AC23" s="7" t="n">
-        <f aca="false">IF(O23="TAK",Arkusz3!$B$22*J23,0)</f>
-        <v>10</v>
+        <f aca="false">IF(O23="TAK",Arkusz3!$B$19*J23,0)</f>
+        <v>5</v>
       </c>
       <c r="AD23" s="7" t="n">
-        <f aca="false">IF(P23="TAK",Arkusz3!$B$23*J23,0)</f>
+        <f aca="false">IF(P23="TAK",Arkusz3!$B$19*J23,0)</f>
         <v>0</v>
       </c>
       <c r="AE23" s="7" t="n">
-        <f aca="false">IF(Q23="TAK",Arkusz3!$B$24*J23,0)</f>
+        <f aca="false">IF(Q23="TAK",Arkusz3!$B$19*J23,0)</f>
         <v>5</v>
       </c>
       <c r="AF23" s="7" t="n">
-        <f aca="false">IF(R23="TAK",Arkusz3!$B$25*J23,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R23="TAK",Arkusz3!$B$19*J23,0)</f>
+        <v>5</v>
       </c>
       <c r="AG23" s="7" t="n">
         <f aca="false">SUM(Z23:AF23)</f>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="AH23" s="7" t="n">
         <f aca="false">IF(L23="Nie",0,5)</f>
@@ -5003,7 +4991,7 @@
       </c>
       <c r="AR23" s="7" t="n">
         <f aca="false">IF(AK23&gt;5,AC23*0.2*(AK23-5)+AC23,AC23)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AS23" s="7" t="n">
         <f aca="false">IF(AL23&gt;5,AD23*0.2*(AL23-5)+AD23,AD23)</f>
@@ -5015,15 +5003,15 @@
       </c>
       <c r="AU23" s="7" t="n">
         <f aca="false">IF(AN23&gt;5,AF23*0.2*(AN23-5)+AF23,AF23)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV23" s="7" t="n">
         <f aca="false">SUM(AO23:AU23)+Y23</f>
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="AW23" s="7" t="n">
         <f aca="false">IF(S23="Roczna",AV23*12*0.95,AV23)</f>
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="AX23" s="7" t="s">
         <v>44</v>
@@ -5116,32 +5104,32 @@
         <v>0</v>
       </c>
       <c r="AA24" s="7" t="n">
-        <f aca="false">IF(M24="TAK",Arkusz3!$B$20*J24,0)</f>
+        <f aca="false">IF(M24="TAK",Arkusz3!$B$19*J24,0)</f>
         <v>0</v>
       </c>
       <c r="AB24" s="7" t="n">
-        <f aca="false">IF(N24="TAK",Arkusz3!$B$21*J24,0)</f>
-        <v>8</v>
+        <f aca="false">IF(N24="TAK",Arkusz3!$B$19*J24,0)</f>
+        <v>5</v>
       </c>
       <c r="AC24" s="7" t="n">
-        <f aca="false">IF(O24="TAK",Arkusz3!$B$22*J24,0)</f>
-        <v>10</v>
+        <f aca="false">IF(O24="TAK",Arkusz3!$B$19*J24,0)</f>
+        <v>5</v>
       </c>
       <c r="AD24" s="7" t="n">
-        <f aca="false">IF(P24="TAK",Arkusz3!$B$23*J24,0)</f>
+        <f aca="false">IF(P24="TAK",Arkusz3!$B$19*J24,0)</f>
         <v>0</v>
       </c>
       <c r="AE24" s="7" t="n">
-        <f aca="false">IF(Q24="TAK",Arkusz3!$B$24*J24,0)</f>
+        <f aca="false">IF(Q24="TAK",Arkusz3!$B$19*J24,0)</f>
         <v>5</v>
       </c>
       <c r="AF24" s="7" t="n">
-        <f aca="false">IF(R24="TAK",Arkusz3!$B$25*J24,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R24="TAK",Arkusz3!$B$19*J24,0)</f>
+        <v>5</v>
       </c>
       <c r="AG24" s="7" t="n">
         <f aca="false">SUM(Z24:AF24)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AH24" s="7" t="n">
         <f aca="false">IF(L24="Nie",0,5)</f>
@@ -5181,11 +5169,11 @@
       </c>
       <c r="AQ24" s="7" t="n">
         <f aca="false">IF(AJ24&gt;5,AB24*0.2*(AJ24-5)+AB24,AB24)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AR24" s="7" t="n">
         <f aca="false">IF(AK24&gt;5,AC24*0.2*(AK24-5)+AC24,AC24)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AS24" s="7" t="n">
         <f aca="false">IF(AL24&gt;5,AD24*0.2*(AL24-5)+AD24,AD24)</f>
@@ -5197,15 +5185,15 @@
       </c>
       <c r="AU24" s="7" t="n">
         <f aca="false">IF(AN24&gt;5,AF24*0.2*(AN24-5)+AF24,AF24)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV24" s="7" t="n">
         <f aca="false">SUM(AO24:AU24)+Y24</f>
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="AW24" s="7" t="n">
         <f aca="false">IF(S24="Roczna",AV24*12*0.95,AV24)</f>
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="AX24" s="7" t="s">
         <v>49</v>
@@ -5298,32 +5286,32 @@
         <v>0</v>
       </c>
       <c r="AA25" s="7" t="n">
-        <f aca="false">IF(M25="TAK",Arkusz3!$B$20*J25,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M25="TAK",Arkusz3!$B$19*J25,0)</f>
+        <v>5</v>
       </c>
       <c r="AB25" s="7" t="n">
-        <f aca="false">IF(N25="TAK",Arkusz3!$B$21*J25,0)</f>
+        <f aca="false">IF(N25="TAK",Arkusz3!$B$19*J25,0)</f>
         <v>0</v>
       </c>
       <c r="AC25" s="7" t="n">
-        <f aca="false">IF(O25="TAK",Arkusz3!$B$22*J25,0)</f>
-        <v>10</v>
+        <f aca="false">IF(O25="TAK",Arkusz3!$B$19*J25,0)</f>
+        <v>5</v>
       </c>
       <c r="AD25" s="7" t="n">
-        <f aca="false">IF(P25="TAK",Arkusz3!$B$23*J25,0)</f>
+        <f aca="false">IF(P25="TAK",Arkusz3!$B$19*J25,0)</f>
         <v>0</v>
       </c>
       <c r="AE25" s="7" t="n">
-        <f aca="false">IF(Q25="TAK",Arkusz3!$B$24*J25,0)</f>
+        <f aca="false">IF(Q25="TAK",Arkusz3!$B$19*J25,0)</f>
         <v>0</v>
       </c>
       <c r="AF25" s="7" t="n">
-        <f aca="false">IF(R25="TAK",Arkusz3!$B$25*J25,0)</f>
+        <f aca="false">IF(R25="TAK",Arkusz3!$B$19*J25,0)</f>
         <v>0</v>
       </c>
       <c r="AG25" s="7" t="n">
         <f aca="false">SUM(Z25:AF25)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AH25" s="7" t="n">
         <f aca="false">IF(L25="Nie",0,5)</f>
@@ -5359,7 +5347,7 @@
       </c>
       <c r="AP25" s="7" t="n">
         <f aca="false">IF(AI25&gt;5,AA25*0.2*(AI25-5)+AA25,AA25)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ25" s="7" t="n">
         <f aca="false">IF(AJ25&gt;5,AB25*0.2*(AJ25-5)+AB25,AB25)</f>
@@ -5367,7 +5355,7 @@
       </c>
       <c r="AR25" s="7" t="n">
         <f aca="false">IF(AK25&gt;5,AC25*0.2*(AK25-5)+AC25,AC25)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AS25" s="7" t="n">
         <f aca="false">IF(AL25&gt;5,AD25*0.2*(AL25-5)+AD25,AD25)</f>
@@ -5383,11 +5371,11 @@
       </c>
       <c r="AV25" s="7" t="n">
         <f aca="false">SUM(AO25:AU25)+Y25</f>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="AW25" s="7" t="n">
         <f aca="false">IF(S25="Roczna",AV25*12*0.95,AV25)</f>
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="AX25" s="7" t="s">
         <v>57</v>
@@ -5480,32 +5468,32 @@
         <v>0</v>
       </c>
       <c r="AA26" s="7" t="n">
-        <f aca="false">IF(M26="TAK",Arkusz3!$B$20*J26,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M26="TAK",Arkusz3!$B$19*J26,0)</f>
+        <v>10</v>
       </c>
       <c r="AB26" s="7" t="n">
-        <f aca="false">IF(N26="TAK",Arkusz3!$B$21*J26,0)</f>
-        <v>16</v>
+        <f aca="false">IF(N26="TAK",Arkusz3!$B$19*J26,0)</f>
+        <v>10</v>
       </c>
       <c r="AC26" s="7" t="n">
-        <f aca="false">IF(O26="TAK",Arkusz3!$B$22*J26,0)</f>
+        <f aca="false">IF(O26="TAK",Arkusz3!$B$19*J26,0)</f>
         <v>0</v>
       </c>
       <c r="AD26" s="7" t="n">
-        <f aca="false">IF(P26="TAK",Arkusz3!$B$23*J26,0)</f>
-        <v>24</v>
+        <f aca="false">IF(P26="TAK",Arkusz3!$B$19*J26,0)</f>
+        <v>10</v>
       </c>
       <c r="AE26" s="7" t="n">
-        <f aca="false">IF(Q26="TAK",Arkusz3!$B$24*J26,0)</f>
+        <f aca="false">IF(Q26="TAK",Arkusz3!$B$19*J26,0)</f>
         <v>0</v>
       </c>
       <c r="AF26" s="7" t="n">
-        <f aca="false">IF(R26="TAK",Arkusz3!$B$25*J26,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R26="TAK",Arkusz3!$B$19*J26,0)</f>
+        <v>10</v>
       </c>
       <c r="AG26" s="7" t="n">
         <f aca="false">SUM(Z26:AF26)</f>
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="AH26" s="7" t="n">
         <f aca="false">IF(L26="Nie",0,5)</f>
@@ -5541,11 +5529,11 @@
       </c>
       <c r="AP26" s="7" t="n">
         <f aca="false">IF(AI26&gt;5,AA26*0.2*(AI26-5)+AA26,AA26)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ26" s="7" t="n">
         <f aca="false">IF(AJ26&gt;5,AB26*0.2*(AJ26-5)+AB26,AB26)</f>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AR26" s="7" t="n">
         <f aca="false">IF(AK26&gt;5,AC26*0.2*(AK26-5)+AC26,AC26)</f>
@@ -5553,7 +5541,7 @@
       </c>
       <c r="AS26" s="7" t="n">
         <f aca="false">IF(AL26&gt;5,AD26*0.2*(AL26-5)+AD26,AD26)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AT26" s="7" t="n">
         <f aca="false">IF(AM26&gt;5,AE26*0.2*(AM26-5)+AE26,AE26)</f>
@@ -5561,15 +5549,15 @@
       </c>
       <c r="AU26" s="7" t="n">
         <f aca="false">IF(AN26&gt;5,AF26*0.2*(AN26-5)+AF26,AF26)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV26" s="7" t="n">
         <f aca="false">SUM(AO26:AU26)+Y26</f>
-        <v>248.5</v>
+        <v>204.5</v>
       </c>
       <c r="AW26" s="7" t="n">
         <f aca="false">IF(S26="Roczna",AV26*12*0.95,AV26)</f>
-        <v>248.5</v>
+        <v>204.5</v>
       </c>
       <c r="AX26" s="7" t="s">
         <v>49</v>
@@ -5662,32 +5650,32 @@
         <v>0</v>
       </c>
       <c r="AA27" s="7" t="n">
-        <f aca="false">IF(M27="TAK",Arkusz3!$B$20*J27,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M27="TAK",Arkusz3!$B$19*J27,0)</f>
+        <v>10</v>
       </c>
       <c r="AB27" s="7" t="n">
-        <f aca="false">IF(N27="TAK",Arkusz3!$B$21*J27,0)</f>
+        <f aca="false">IF(N27="TAK",Arkusz3!$B$19*J27,0)</f>
         <v>0</v>
       </c>
       <c r="AC27" s="7" t="n">
-        <f aca="false">IF(O27="TAK",Arkusz3!$B$22*J27,0)</f>
-        <v>20</v>
+        <f aca="false">IF(O27="TAK",Arkusz3!$B$19*J27,0)</f>
+        <v>10</v>
       </c>
       <c r="AD27" s="7" t="n">
-        <f aca="false">IF(P27="TAK",Arkusz3!$B$23*J27,0)</f>
+        <f aca="false">IF(P27="TAK",Arkusz3!$B$19*J27,0)</f>
         <v>0</v>
       </c>
       <c r="AE27" s="7" t="n">
-        <f aca="false">IF(Q27="TAK",Arkusz3!$B$24*J27,0)</f>
+        <f aca="false">IF(Q27="TAK",Arkusz3!$B$19*J27,0)</f>
         <v>10</v>
       </c>
       <c r="AF27" s="7" t="n">
-        <f aca="false">IF(R27="TAK",Arkusz3!$B$25*J27,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R27="TAK",Arkusz3!$B$19*J27,0)</f>
+        <v>10</v>
       </c>
       <c r="AG27" s="7" t="n">
         <f aca="false">SUM(Z27:AF27)</f>
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="AH27" s="7" t="n">
         <f aca="false">IF(L27="Nie",0,5)</f>
@@ -5722,7 +5710,7 @@
       </c>
       <c r="AP27" s="7" t="n">
         <f aca="false">IF(AI27&gt;5,AA27*0.2*(AI27-5)+AA27,AA27)</f>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="AQ27" s="7" t="n">
         <f aca="false">IF(AJ27&gt;5,AB27*0.2*(AJ27-5)+AB27,AB27)</f>
@@ -5730,7 +5718,7 @@
       </c>
       <c r="AR27" s="7" t="n">
         <f aca="false">IF(AK27&gt;5,AC27*0.2*(AK27-5)+AC27,AC27)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS27" s="7" t="n">
         <f aca="false">IF(AL27&gt;5,AD27*0.2*(AL27-5)+AD27,AD27)</f>
@@ -5742,15 +5730,15 @@
       </c>
       <c r="AU27" s="7" t="n">
         <f aca="false">IF(AN27&gt;5,AF27*0.2*(AN27-5)+AF27,AF27)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV27" s="7" t="n">
         <f aca="false">SUM(AO27:AU27)+Y27</f>
-        <v>253.5</v>
+        <v>209.5</v>
       </c>
       <c r="AW27" s="7" t="n">
         <f aca="false">IF(S27="Roczna",AV27*12*0.95,AV27)</f>
-        <v>253.5</v>
+        <v>209.5</v>
       </c>
       <c r="AX27" s="7" t="s">
         <v>57</v>
@@ -5843,32 +5831,32 @@
         <v>5</v>
       </c>
       <c r="AA28" s="7" t="n">
-        <f aca="false">IF(M28="TAK",Arkusz3!$B$20*J28,0)</f>
+        <f aca="false">IF(M28="TAK",Arkusz3!$B$19*J28,0)</f>
         <v>0</v>
       </c>
       <c r="AB28" s="7" t="n">
-        <f aca="false">IF(N28="TAK",Arkusz3!$B$21*J28,0)</f>
+        <f aca="false">IF(N28="TAK",Arkusz3!$B$19*J28,0)</f>
         <v>0</v>
       </c>
       <c r="AC28" s="7" t="n">
-        <f aca="false">IF(O28="TAK",Arkusz3!$B$22*J28,0)</f>
+        <f aca="false">IF(O28="TAK",Arkusz3!$B$19*J28,0)</f>
         <v>0</v>
       </c>
       <c r="AD28" s="7" t="n">
-        <f aca="false">IF(P28="TAK",Arkusz3!$B$23*J28,0)</f>
+        <f aca="false">IF(P28="TAK",Arkusz3!$B$19*J28,0)</f>
         <v>0</v>
       </c>
       <c r="AE28" s="7" t="n">
-        <f aca="false">IF(Q28="TAK",Arkusz3!$B$24*J28,0)</f>
+        <f aca="false">IF(Q28="TAK",Arkusz3!$B$19*J28,0)</f>
         <v>5</v>
       </c>
       <c r="AF28" s="7" t="n">
-        <f aca="false">IF(R28="TAK",Arkusz3!$B$25*J28,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R28="TAK",Arkusz3!$B$19*J28,0)</f>
+        <v>5</v>
       </c>
       <c r="AG28" s="7" t="n">
         <f aca="false">SUM(Z28:AF28)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AH28" s="7" t="n">
         <f aca="false">IF(L28="Nie",0,5)</f>
@@ -5924,15 +5912,15 @@
       </c>
       <c r="AU28" s="7" t="n">
         <f aca="false">IF(AN28&gt;5,AF28*0.2*(AN28-5)+AF28,AF28)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV28" s="7" t="n">
         <f aca="false">SUM(AO28:AU28)+Y28</f>
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AW28" s="7" t="n">
         <f aca="false">IF(S28="Roczna",AV28*12*0.95,AV28)</f>
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AX28" s="7" t="s">
         <v>44</v>
@@ -6025,32 +6013,32 @@
         <v>5</v>
       </c>
       <c r="AA29" s="7" t="n">
-        <f aca="false">IF(M29="TAK",Arkusz3!$B$20*J29,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M29="TAK",Arkusz3!$B$19*J29,0)</f>
+        <v>5</v>
       </c>
       <c r="AB29" s="7" t="n">
-        <f aca="false">IF(N29="TAK",Arkusz3!$B$21*J29,0)</f>
+        <f aca="false">IF(N29="TAK",Arkusz3!$B$19*J29,0)</f>
         <v>0</v>
       </c>
       <c r="AC29" s="7" t="n">
-        <f aca="false">IF(O29="TAK",Arkusz3!$B$22*J29,0)</f>
+        <f aca="false">IF(O29="TAK",Arkusz3!$B$19*J29,0)</f>
         <v>0</v>
       </c>
       <c r="AD29" s="7" t="n">
-        <f aca="false">IF(P29="TAK",Arkusz3!$B$23*J29,0)</f>
-        <v>12</v>
+        <f aca="false">IF(P29="TAK",Arkusz3!$B$19*J29,0)</f>
+        <v>5</v>
       </c>
       <c r="AE29" s="7" t="n">
-        <f aca="false">IF(Q29="TAK",Arkusz3!$B$24*J29,0)</f>
+        <f aca="false">IF(Q29="TAK",Arkusz3!$B$19*J29,0)</f>
         <v>5</v>
       </c>
       <c r="AF29" s="7" t="n">
-        <f aca="false">IF(R29="TAK",Arkusz3!$B$25*J29,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R29="TAK",Arkusz3!$B$19*J29,0)</f>
+        <v>5</v>
       </c>
       <c r="AG29" s="7" t="n">
         <f aca="false">SUM(Z29:AF29)</f>
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="AH29" s="7" t="n">
         <f aca="false">IF(L29="Nie",0,5)</f>
@@ -6086,7 +6074,7 @@
       </c>
       <c r="AP29" s="7" t="n">
         <f aca="false">IF(AI29&gt;5,AA29*0.2*(AI29-5)+AA29,AA29)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ29" s="7" t="n">
         <f aca="false">IF(AJ29&gt;5,AB29*0.2*(AJ29-5)+AB29,AB29)</f>
@@ -6098,7 +6086,7 @@
       </c>
       <c r="AS29" s="7" t="n">
         <f aca="false">IF(AL29&gt;5,AD29*0.2*(AL29-5)+AD29,AD29)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AT29" s="7" t="n">
         <f aca="false">IF(AM29&gt;5,AE29*0.2*(AM29-5)+AE29,AE29)</f>
@@ -6106,15 +6094,15 @@
       </c>
       <c r="AU29" s="7" t="n">
         <f aca="false">IF(AN29&gt;5,AF29*0.2*(AN29-5)+AF29,AF29)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV29" s="7" t="n">
         <f aca="false">SUM(AO29:AU29)+Y29</f>
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="AW29" s="7" t="n">
         <f aca="false">IF(S29="Roczna",AV29*12*0.95,AV29)</f>
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="AX29" s="7" t="s">
         <v>44</v>
@@ -6207,32 +6195,32 @@
         <v>0</v>
       </c>
       <c r="AA30" s="7" t="n">
-        <f aca="false">IF(M30="TAK",Arkusz3!$B$20*J30,0)</f>
+        <f aca="false">IF(M30="TAK",Arkusz3!$B$19*J30,0)</f>
         <v>0</v>
       </c>
       <c r="AB30" s="7" t="n">
-        <f aca="false">IF(N30="TAK",Arkusz3!$B$21*J30,0)</f>
+        <f aca="false">IF(N30="TAK",Arkusz3!$B$19*J30,0)</f>
         <v>0</v>
       </c>
       <c r="AC30" s="7" t="n">
-        <f aca="false">IF(O30="TAK",Arkusz3!$B$22*J30,0)</f>
-        <v>20</v>
+        <f aca="false">IF(O30="TAK",Arkusz3!$B$19*J30,0)</f>
+        <v>10</v>
       </c>
       <c r="AD30" s="7" t="n">
-        <f aca="false">IF(P30="TAK",Arkusz3!$B$23*J30,0)</f>
+        <f aca="false">IF(P30="TAK",Arkusz3!$B$19*J30,0)</f>
         <v>0</v>
       </c>
       <c r="AE30" s="7" t="n">
-        <f aca="false">IF(Q30="TAK",Arkusz3!$B$24*J30,0)</f>
+        <f aca="false">IF(Q30="TAK",Arkusz3!$B$19*J30,0)</f>
         <v>0</v>
       </c>
       <c r="AF30" s="7" t="n">
-        <f aca="false">IF(R30="TAK",Arkusz3!$B$25*J30,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R30="TAK",Arkusz3!$B$19*J30,0)</f>
+        <v>10</v>
       </c>
       <c r="AG30" s="7" t="n">
         <f aca="false">SUM(Z30:AF30)</f>
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="AH30" s="7" t="n">
         <f aca="false">IF(L30="Nie",0,5)</f>
@@ -6276,7 +6264,7 @@
       </c>
       <c r="AR30" s="7" t="n">
         <f aca="false">IF(AK30&gt;5,AC30*0.2*(AK30-5)+AC30,AC30)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS30" s="7" t="n">
         <f aca="false">IF(AL30&gt;5,AD30*0.2*(AL30-5)+AD30,AD30)</f>
@@ -6288,15 +6276,15 @@
       </c>
       <c r="AU30" s="7" t="n">
         <f aca="false">IF(AN30&gt;5,AF30*0.2*(AN30-5)+AF30,AF30)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV30" s="7" t="n">
         <f aca="false">SUM(AO30:AU30)+Y30</f>
-        <v>428.5</v>
+        <v>404.5</v>
       </c>
       <c r="AW30" s="7" t="n">
         <f aca="false">IF(S30="Roczna",AV30*12*0.95,AV30)</f>
-        <v>428.5</v>
+        <v>404.5</v>
       </c>
       <c r="AX30" s="7" t="s">
         <v>44</v>
@@ -6389,32 +6377,32 @@
         <v>5</v>
       </c>
       <c r="AA31" s="7" t="n">
-        <f aca="false">IF(M31="TAK",Arkusz3!$B$20*J31,0)</f>
+        <f aca="false">IF(M31="TAK",Arkusz3!$B$19*J31,0)</f>
         <v>0</v>
       </c>
       <c r="AB31" s="7" t="n">
-        <f aca="false">IF(N31="TAK",Arkusz3!$B$21*J31,0)</f>
+        <f aca="false">IF(N31="TAK",Arkusz3!$B$19*J31,0)</f>
         <v>0</v>
       </c>
       <c r="AC31" s="7" t="n">
-        <f aca="false">IF(O31="TAK",Arkusz3!$B$22*J31,0)</f>
+        <f aca="false">IF(O31="TAK",Arkusz3!$B$19*J31,0)</f>
         <v>0</v>
       </c>
       <c r="AD31" s="7" t="n">
-        <f aca="false">IF(P31="TAK",Arkusz3!$B$23*J31,0)</f>
+        <f aca="false">IF(P31="TAK",Arkusz3!$B$19*J31,0)</f>
         <v>0</v>
       </c>
       <c r="AE31" s="7" t="n">
-        <f aca="false">IF(Q31="TAK",Arkusz3!$B$24*J31,0)</f>
+        <f aca="false">IF(Q31="TAK",Arkusz3!$B$19*J31,0)</f>
         <v>5</v>
       </c>
       <c r="AF31" s="7" t="n">
-        <f aca="false">IF(R31="TAK",Arkusz3!$B$25*J31,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R31="TAK",Arkusz3!$B$19*J31,0)</f>
+        <v>5</v>
       </c>
       <c r="AG31" s="7" t="n">
         <f aca="false">SUM(Z31:AF31)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AH31" s="7" t="n">
         <v>10</v>
@@ -6467,15 +6455,15 @@
       </c>
       <c r="AU31" s="7" t="n">
         <f aca="false">IF(AN31&gt;5,AF31*0.2*(AN31-5)+AF31,AF31)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV31" s="7" t="n">
         <f aca="false">SUM(AO31:AU31)+Y31</f>
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="AW31" s="7" t="n">
         <f aca="false">IF(S31="Roczna",AV31*12*0.95,AV31)</f>
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="AX31" s="7" t="s">
         <v>49</v>
@@ -6568,32 +6556,32 @@
         <v>0</v>
       </c>
       <c r="AA32" s="7" t="n">
-        <f aca="false">IF(M32="TAK",Arkusz3!$B$20*J32,0)</f>
+        <f aca="false">IF(M32="TAK",Arkusz3!$B$19*J32,0)</f>
         <v>0</v>
       </c>
       <c r="AB32" s="7" t="n">
-        <f aca="false">IF(N32="TAK",Arkusz3!$B$21*J32,0)</f>
+        <f aca="false">IF(N32="TAK",Arkusz3!$B$19*J32,0)</f>
         <v>0</v>
       </c>
       <c r="AC32" s="7" t="n">
-        <f aca="false">IF(O32="TAK",Arkusz3!$B$22*J32,0)</f>
-        <v>10</v>
+        <f aca="false">IF(O32="TAK",Arkusz3!$B$19*J32,0)</f>
+        <v>5</v>
       </c>
       <c r="AD32" s="7" t="n">
-        <f aca="false">IF(P32="TAK",Arkusz3!$B$23*J32,0)</f>
+        <f aca="false">IF(P32="TAK",Arkusz3!$B$19*J32,0)</f>
         <v>0</v>
       </c>
       <c r="AE32" s="7" t="n">
-        <f aca="false">IF(Q32="TAK",Arkusz3!$B$24*J32,0)</f>
+        <f aca="false">IF(Q32="TAK",Arkusz3!$B$19*J32,0)</f>
         <v>0</v>
       </c>
       <c r="AF32" s="7" t="n">
-        <f aca="false">IF(R32="TAK",Arkusz3!$B$25*J32,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R32="TAK",Arkusz3!$B$19*J32,0)</f>
+        <v>5</v>
       </c>
       <c r="AG32" s="7" t="n">
         <f aca="false">SUM(Z32:AF32)</f>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="AH32" s="7" t="n">
         <f aca="false">IF(L32="Nie",0,5)</f>
@@ -6637,7 +6625,7 @@
       </c>
       <c r="AR32" s="7" t="n">
         <f aca="false">IF(AK32&gt;5,AC32*0.2*(AK32-5)+AC32,AC32)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AS32" s="7" t="n">
         <f aca="false">IF(AL32&gt;5,AD32*0.2*(AL32-5)+AD32,AD32)</f>
@@ -6649,15 +6637,15 @@
       </c>
       <c r="AU32" s="7" t="n">
         <f aca="false">IF(AN32&gt;5,AF32*0.2*(AN32-5)+AF32,AF32)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV32" s="7" t="n">
         <f aca="false">SUM(AO32:AU32)+Y32</f>
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="AW32" s="7" t="n">
         <f aca="false">IF(S32="Roczna",AV32*12*0.95,AV32)</f>
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="AX32" s="7" t="s">
         <v>57</v>
@@ -6750,32 +6738,32 @@
         <v>0</v>
       </c>
       <c r="AA33" s="7" t="n">
-        <f aca="false">IF(M33="TAK",Arkusz3!$B$20*J33,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M33="TAK",Arkusz3!$B$19*J33,0)</f>
+        <v>10</v>
       </c>
       <c r="AB33" s="7" t="n">
-        <f aca="false">IF(N33="TAK",Arkusz3!$B$21*J33,0)</f>
+        <f aca="false">IF(N33="TAK",Arkusz3!$B$19*J33,0)</f>
         <v>0</v>
       </c>
       <c r="AC33" s="7" t="n">
-        <f aca="false">IF(O33="TAK",Arkusz3!$B$22*J33,0)</f>
+        <f aca="false">IF(O33="TAK",Arkusz3!$B$19*J33,0)</f>
         <v>0</v>
       </c>
       <c r="AD33" s="7" t="n">
-        <f aca="false">IF(P33="TAK",Arkusz3!$B$23*J33,0)</f>
+        <f aca="false">IF(P33="TAK",Arkusz3!$B$19*J33,0)</f>
         <v>0</v>
       </c>
       <c r="AE33" s="7" t="n">
-        <f aca="false">IF(Q33="TAK",Arkusz3!$B$24*J33,0)</f>
+        <f aca="false">IF(Q33="TAK",Arkusz3!$B$19*J33,0)</f>
         <v>10</v>
       </c>
       <c r="AF33" s="7" t="n">
-        <f aca="false">IF(R33="TAK",Arkusz3!$B$25*J33,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R33="TAK",Arkusz3!$B$19*J33,0)</f>
+        <v>10</v>
       </c>
       <c r="AG33" s="7" t="n">
         <f aca="false">SUM(Z33:AF33)</f>
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="AH33" s="7" t="n">
         <f aca="false">IF(L33="Nie",0,5)</f>
@@ -6811,7 +6799,7 @@
       </c>
       <c r="AP33" s="7" t="n">
         <f aca="false">IF(AI33&gt;5,AA33*0.2*(AI33-5)+AA33,AA33)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ33" s="7" t="n">
         <f aca="false">IF(AJ33&gt;5,AB33*0.2*(AJ33-5)+AB33,AB33)</f>
@@ -6831,15 +6819,15 @@
       </c>
       <c r="AU33" s="7" t="n">
         <f aca="false">IF(AN33&gt;5,AF33*0.2*(AN33-5)+AF33,AF33)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV33" s="7" t="n">
         <f aca="false">SUM(AO33:AU33)+Y33</f>
-        <v>188.5</v>
+        <v>164.5</v>
       </c>
       <c r="AW33" s="7" t="n">
         <f aca="false">IF(S33="Roczna",AV33*12*0.95,AV33)</f>
-        <v>188.5</v>
+        <v>164.5</v>
       </c>
       <c r="AX33" s="7" t="s">
         <v>49</v>
@@ -6932,32 +6920,32 @@
         <v>0</v>
       </c>
       <c r="AA34" s="7" t="n">
-        <f aca="false">IF(M34="TAK",Arkusz3!$B$20*J34,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M34="TAK",Arkusz3!$B$19*J34,0)</f>
+        <v>5</v>
       </c>
       <c r="AB34" s="7" t="n">
-        <f aca="false">IF(N34="TAK",Arkusz3!$B$21*J34,0)</f>
-        <v>8</v>
+        <f aca="false">IF(N34="TAK",Arkusz3!$B$19*J34,0)</f>
+        <v>5</v>
       </c>
       <c r="AC34" s="7" t="n">
-        <f aca="false">IF(O34="TAK",Arkusz3!$B$22*J34,0)</f>
+        <f aca="false">IF(O34="TAK",Arkusz3!$B$19*J34,0)</f>
         <v>0</v>
       </c>
       <c r="AD34" s="7" t="n">
-        <f aca="false">IF(P34="TAK",Arkusz3!$B$23*J34,0)</f>
-        <v>12</v>
+        <f aca="false">IF(P34="TAK",Arkusz3!$B$19*J34,0)</f>
+        <v>5</v>
       </c>
       <c r="AE34" s="7" t="n">
-        <f aca="false">IF(Q34="TAK",Arkusz3!$B$24*J34,0)</f>
+        <f aca="false">IF(Q34="TAK",Arkusz3!$B$19*J34,0)</f>
         <v>0</v>
       </c>
       <c r="AF34" s="7" t="n">
-        <f aca="false">IF(R34="TAK",Arkusz3!$B$25*J34,0)</f>
+        <f aca="false">IF(R34="TAK",Arkusz3!$B$19*J34,0)</f>
         <v>0</v>
       </c>
       <c r="AG34" s="7" t="n">
         <f aca="false">SUM(Z34:AF34)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AH34" s="7" t="n">
         <f aca="false">IF(L34="Nie",0,5)</f>
@@ -6993,11 +6981,11 @@
       </c>
       <c r="AP34" s="7" t="n">
         <f aca="false">IF(AI34&gt;5,AA34*0.2*(AI34-5)+AA34,AA34)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ34" s="7" t="n">
         <f aca="false">IF(AJ34&gt;5,AB34*0.2*(AJ34-5)+AB34,AB34)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AR34" s="7" t="n">
         <f aca="false">IF(AK34&gt;5,AC34*0.2*(AK34-5)+AC34,AC34)</f>
@@ -7005,7 +6993,7 @@
       </c>
       <c r="AS34" s="7" t="n">
         <f aca="false">IF(AL34&gt;5,AD34*0.2*(AL34-5)+AD34,AD34)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AT34" s="7" t="n">
         <f aca="false">IF(AM34&gt;5,AE34*0.2*(AM34-5)+AE34,AE34)</f>
@@ -7017,11 +7005,11 @@
       </c>
       <c r="AV34" s="7" t="n">
         <f aca="false">SUM(AO34:AU34)+Y34</f>
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="AW34" s="7" t="n">
         <f aca="false">IF(S34="Roczna",AV34*12*0.95,AV34)</f>
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="AX34" s="7" t="s">
         <v>49</v>
@@ -7114,32 +7102,32 @@
         <v>0</v>
       </c>
       <c r="AA35" s="7" t="n">
-        <f aca="false">IF(M35="TAK",Arkusz3!$B$20*J35,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M35="TAK",Arkusz3!$B$19*J35,0)</f>
+        <v>5</v>
       </c>
       <c r="AB35" s="7" t="n">
-        <f aca="false">IF(N35="TAK",Arkusz3!$B$21*J35,0)</f>
+        <f aca="false">IF(N35="TAK",Arkusz3!$B$19*J35,0)</f>
         <v>0</v>
       </c>
       <c r="AC35" s="7" t="n">
-        <f aca="false">IF(O35="TAK",Arkusz3!$B$22*J35,0)</f>
+        <f aca="false">IF(O35="TAK",Arkusz3!$B$19*J35,0)</f>
         <v>0</v>
       </c>
       <c r="AD35" s="7" t="n">
-        <f aca="false">IF(P35="TAK",Arkusz3!$B$23*J35,0)</f>
+        <f aca="false">IF(P35="TAK",Arkusz3!$B$19*J35,0)</f>
         <v>0</v>
       </c>
       <c r="AE35" s="7" t="n">
-        <f aca="false">IF(Q35="TAK",Arkusz3!$B$24*J35,0)</f>
+        <f aca="false">IF(Q35="TAK",Arkusz3!$B$19*J35,0)</f>
         <v>5</v>
       </c>
       <c r="AF35" s="7" t="n">
-        <f aca="false">IF(R35="TAK",Arkusz3!$B$25*J35,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R35="TAK",Arkusz3!$B$19*J35,0)</f>
+        <v>5</v>
       </c>
       <c r="AG35" s="7" t="n">
         <f aca="false">SUM(Z35:AF35)</f>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="AH35" s="7" t="n">
         <f aca="false">IF(L35="Nie",0,5)</f>
@@ -7175,7 +7163,7 @@
       </c>
       <c r="AP35" s="7" t="n">
         <f aca="false">IF(AI35&gt;5,AA35*0.2*(AI35-5)+AA35,AA35)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ35" s="7" t="n">
         <f aca="false">IF(AJ35&gt;5,AB35*0.2*(AJ35-5)+AB35,AB35)</f>
@@ -7195,15 +7183,15 @@
       </c>
       <c r="AU35" s="7" t="n">
         <f aca="false">IF(AN35&gt;5,AF35*0.2*(AN35-5)+AF35,AF35)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV35" s="7" t="n">
         <f aca="false">SUM(AO35:AU35)+Y35</f>
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AW35" s="7" t="n">
         <f aca="false">IF(S35="Roczna",AV35*12*0.95,AV35)</f>
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="AX35" s="7" t="s">
         <v>44</v>
@@ -7296,32 +7284,32 @@
         <v>0</v>
       </c>
       <c r="AA36" s="7" t="n">
-        <f aca="false">IF(M36="TAK",Arkusz3!$B$20*J36,0)</f>
-        <v>20</v>
+        <f aca="false">IF(M36="TAK",Arkusz3!$B$19*J36,0)</f>
+        <v>10</v>
       </c>
       <c r="AB36" s="7" t="n">
-        <f aca="false">IF(N36="TAK",Arkusz3!$B$21*J36,0)</f>
-        <v>16</v>
+        <f aca="false">IF(N36="TAK",Arkusz3!$B$19*J36,0)</f>
+        <v>10</v>
       </c>
       <c r="AC36" s="7" t="n">
-        <f aca="false">IF(O36="TAK",Arkusz3!$B$22*J36,0)</f>
+        <f aca="false">IF(O36="TAK",Arkusz3!$B$19*J36,0)</f>
         <v>0</v>
       </c>
       <c r="AD36" s="7" t="n">
-        <f aca="false">IF(P36="TAK",Arkusz3!$B$23*J36,0)</f>
-        <v>24</v>
+        <f aca="false">IF(P36="TAK",Arkusz3!$B$19*J36,0)</f>
+        <v>10</v>
       </c>
       <c r="AE36" s="7" t="n">
-        <f aca="false">IF(Q36="TAK",Arkusz3!$B$24*J36,0)</f>
+        <f aca="false">IF(Q36="TAK",Arkusz3!$B$19*J36,0)</f>
         <v>0</v>
       </c>
       <c r="AF36" s="7" t="n">
-        <f aca="false">IF(R36="TAK",Arkusz3!$B$25*J36,0)</f>
+        <f aca="false">IF(R36="TAK",Arkusz3!$B$19*J36,0)</f>
         <v>0</v>
       </c>
       <c r="AG36" s="7" t="n">
         <f aca="false">SUM(Z36:AF36)</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="AH36" s="7" t="n">
         <f aca="false">IF(L36="Nie",0,5)</f>
@@ -7357,11 +7345,11 @@
       </c>
       <c r="AP36" s="7" t="n">
         <f aca="false">IF(AI36&gt;5,AA36*0.2*(AI36-5)+AA36,AA36)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AQ36" s="7" t="n">
         <f aca="false">IF(AJ36&gt;5,AB36*0.2*(AJ36-5)+AB36,AB36)</f>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AR36" s="7" t="n">
         <f aca="false">IF(AK36&gt;5,AC36*0.2*(AK36-5)+AC36,AC36)</f>
@@ -7369,7 +7357,7 @@
       </c>
       <c r="AS36" s="7" t="n">
         <f aca="false">IF(AL36&gt;5,AD36*0.2*(AL36-5)+AD36,AD36)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AT36" s="7" t="n">
         <f aca="false">IF(AM36&gt;5,AE36*0.2*(AM36-5)+AE36,AE36)</f>
@@ -7381,11 +7369,11 @@
       </c>
       <c r="AV36" s="7" t="n">
         <f aca="false">SUM(AO36:AU36)+Y36</f>
-        <v>244.5</v>
+        <v>214.5</v>
       </c>
       <c r="AW36" s="7" t="n">
         <f aca="false">IF(S36="Roczna",AV36*12*0.95,AV36)</f>
-        <v>2787.3</v>
+        <v>2445.3</v>
       </c>
       <c r="AX36" s="7" t="s">
         <v>44</v>
@@ -7478,32 +7466,32 @@
         <v>5</v>
       </c>
       <c r="AA37" s="7" t="n">
-        <f aca="false">IF(M37="TAK",Arkusz3!$B$20*J37,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M37="TAK",Arkusz3!$B$19*J37,0)</f>
+        <v>5</v>
       </c>
       <c r="AB37" s="7" t="n">
-        <f aca="false">IF(N37="TAK",Arkusz3!$B$21*J37,0)</f>
+        <f aca="false">IF(N37="TAK",Arkusz3!$B$19*J37,0)</f>
         <v>0</v>
       </c>
       <c r="AC37" s="7" t="n">
-        <f aca="false">IF(O37="TAK",Arkusz3!$B$22*J37,0)</f>
+        <f aca="false">IF(O37="TAK",Arkusz3!$B$19*J37,0)</f>
         <v>0</v>
       </c>
       <c r="AD37" s="7" t="n">
-        <f aca="false">IF(P37="TAK",Arkusz3!$B$23*J37,0)</f>
+        <f aca="false">IF(P37="TAK",Arkusz3!$B$19*J37,0)</f>
         <v>0</v>
       </c>
       <c r="AE37" s="7" t="n">
-        <f aca="false">IF(Q37="TAK",Arkusz3!$B$24*J37,0)</f>
+        <f aca="false">IF(Q37="TAK",Arkusz3!$B$19*J37,0)</f>
         <v>5</v>
       </c>
       <c r="AF37" s="7" t="n">
-        <f aca="false">IF(R37="TAK",Arkusz3!$B$25*J37,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R37="TAK",Arkusz3!$B$19*J37,0)</f>
+        <v>5</v>
       </c>
       <c r="AG37" s="7" t="n">
         <f aca="false">SUM(Z37:AF37)</f>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="AH37" s="7" t="n">
         <f aca="false">IF(L37="Nie",0,5)</f>
@@ -7539,7 +7527,7 @@
       </c>
       <c r="AP37" s="7" t="n">
         <f aca="false">IF(AI37&gt;5,AA37*0.2*(AI37-5)+AA37,AA37)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ37" s="7" t="n">
         <f aca="false">IF(AJ37&gt;5,AB37*0.2*(AJ37-5)+AB37,AB37)</f>
@@ -7559,15 +7547,15 @@
       </c>
       <c r="AU37" s="7" t="n">
         <f aca="false">IF(AN37&gt;5,AF37*0.2*(AN37-5)+AF37,AF37)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV37" s="7" t="n">
         <f aca="false">SUM(AO37:AU37)+Y37</f>
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="AW37" s="7" t="n">
         <f aca="false">IF(S37="Roczna",AV37*12*0.95,AV37)</f>
-        <v>820.8</v>
+        <v>684</v>
       </c>
       <c r="AX37" s="7" t="s">
         <v>57</v>
@@ -7660,32 +7648,32 @@
         <v>5</v>
       </c>
       <c r="AA38" s="7" t="n">
-        <f aca="false">IF(M38="TAK",Arkusz3!$B$20*J38,0)</f>
+        <f aca="false">IF(M38="TAK",Arkusz3!$B$19*J38,0)</f>
         <v>0</v>
       </c>
       <c r="AB38" s="7" t="n">
-        <f aca="false">IF(N38="TAK",Arkusz3!$B$21*J38,0)</f>
+        <f aca="false">IF(N38="TAK",Arkusz3!$B$19*J38,0)</f>
         <v>0</v>
       </c>
       <c r="AC38" s="7" t="n">
-        <f aca="false">IF(O38="TAK",Arkusz3!$B$22*J38,0)</f>
+        <f aca="false">IF(O38="TAK",Arkusz3!$B$19*J38,0)</f>
         <v>0</v>
       </c>
       <c r="AD38" s="7" t="n">
-        <f aca="false">IF(P38="TAK",Arkusz3!$B$23*J38,0)</f>
+        <f aca="false">IF(P38="TAK",Arkusz3!$B$19*J38,0)</f>
         <v>0</v>
       </c>
       <c r="AE38" s="7" t="n">
-        <f aca="false">IF(Q38="TAK",Arkusz3!$B$24*J38,0)</f>
+        <f aca="false">IF(Q38="TAK",Arkusz3!$B$19*J38,0)</f>
         <v>5</v>
       </c>
       <c r="AF38" s="7" t="n">
-        <f aca="false">IF(R38="TAK",Arkusz3!$B$25*J38,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R38="TAK",Arkusz3!$B$19*J38,0)</f>
+        <v>5</v>
       </c>
       <c r="AG38" s="7" t="n">
         <f aca="false">SUM(Z38:AF38)</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AH38" s="7" t="n">
         <f aca="false">IF(L38="Nie",0,5)</f>
@@ -7741,15 +7729,15 @@
       </c>
       <c r="AU38" s="7" t="n">
         <f aca="false">IF(AN38&gt;5,AF38*0.2*(AN38-5)+AF38,AF38)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV38" s="7" t="n">
         <f aca="false">SUM(AO38:AU38)+Y38</f>
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="AW38" s="7" t="n">
         <f aca="false">IF(S38="Roczna",AV38*12*0.95,AV38)</f>
-        <v>1618.8</v>
+        <v>1539</v>
       </c>
       <c r="AX38" s="7" t="s">
         <v>57</v>
@@ -7842,32 +7830,32 @@
         <v>0</v>
       </c>
       <c r="AA39" s="7" t="n">
-        <f aca="false">IF(M39="TAK",Arkusz3!$B$20*J39,0)</f>
+        <f aca="false">IF(M39="TAK",Arkusz3!$B$19*J39,0)</f>
         <v>0</v>
       </c>
       <c r="AB39" s="7" t="n">
-        <f aca="false">IF(N39="TAK",Arkusz3!$B$21*J39,0)</f>
-        <v>16</v>
+        <f aca="false">IF(N39="TAK",Arkusz3!$B$19*J39,0)</f>
+        <v>10</v>
       </c>
       <c r="AC39" s="7" t="n">
-        <f aca="false">IF(O39="TAK",Arkusz3!$B$22*J39,0)</f>
-        <v>20</v>
+        <f aca="false">IF(O39="TAK",Arkusz3!$B$19*J39,0)</f>
+        <v>10</v>
       </c>
       <c r="AD39" s="7" t="n">
-        <f aca="false">IF(P39="TAK",Arkusz3!$B$23*J39,0)</f>
-        <v>24</v>
+        <f aca="false">IF(P39="TAK",Arkusz3!$B$19*J39,0)</f>
+        <v>10</v>
       </c>
       <c r="AE39" s="7" t="n">
-        <f aca="false">IF(Q39="TAK",Arkusz3!$B$24*J39,0)</f>
+        <f aca="false">IF(Q39="TAK",Arkusz3!$B$19*J39,0)</f>
         <v>10</v>
       </c>
       <c r="AF39" s="7" t="n">
-        <f aca="false">IF(R39="TAK",Arkusz3!$B$25*J39,0)</f>
-        <v>24</v>
+        <f aca="false">IF(R39="TAK",Arkusz3!$B$19*J39,0)</f>
+        <v>10</v>
       </c>
       <c r="AG39" s="7" t="n">
         <f aca="false">SUM(Z39:AF39)</f>
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="AH39" s="7" t="n">
         <f aca="false">IF(L39="Nie",0,5)</f>
@@ -7907,15 +7895,15 @@
       </c>
       <c r="AQ39" s="7" t="n">
         <f aca="false">IF(AJ39&gt;5,AB39*0.2*(AJ39-5)+AB39,AB39)</f>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AR39" s="7" t="n">
         <f aca="false">IF(AK39&gt;5,AC39*0.2*(AK39-5)+AC39,AC39)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS39" s="7" t="n">
         <f aca="false">IF(AL39&gt;5,AD39*0.2*(AL39-5)+AD39,AD39)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AT39" s="7" t="n">
         <f aca="false">IF(AM39&gt;5,AE39*0.2*(AM39-5)+AE39,AE39)</f>
@@ -7923,15 +7911,15 @@
       </c>
       <c r="AU39" s="7" t="n">
         <f aca="false">IF(AN39&gt;5,AF39*0.2*(AN39-5)+AF39,AF39)</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="AV39" s="7" t="n">
         <f aca="false">SUM(AO39:AU39)+Y39</f>
-        <v>228.5</v>
+        <v>184.5</v>
       </c>
       <c r="AW39" s="7" t="n">
         <f aca="false">IF(S39="Roczna",AV39*12*0.95,AV39)</f>
-        <v>228.5</v>
+        <v>184.5</v>
       </c>
       <c r="AX39" s="7" t="s">
         <v>44</v>
@@ -8024,32 +8012,32 @@
         <v>0</v>
       </c>
       <c r="AA40" s="7" t="n">
-        <f aca="false">IF(M40="TAK",Arkusz3!$B$20*J40,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M40="TAK",Arkusz3!$B$19*J40,0)</f>
+        <v>5</v>
       </c>
       <c r="AB40" s="7" t="n">
-        <f aca="false">IF(N40="TAK",Arkusz3!$B$21*J40,0)</f>
+        <f aca="false">IF(N40="TAK",Arkusz3!$B$19*J40,0)</f>
         <v>0</v>
       </c>
       <c r="AC40" s="7" t="n">
-        <f aca="false">IF(O40="TAK",Arkusz3!$B$22*J40,0)</f>
+        <f aca="false">IF(O40="TAK",Arkusz3!$B$19*J40,0)</f>
         <v>0</v>
       </c>
       <c r="AD40" s="7" t="n">
-        <f aca="false">IF(P40="TAK",Arkusz3!$B$23*J40,0)</f>
+        <f aca="false">IF(P40="TAK",Arkusz3!$B$19*J40,0)</f>
         <v>0</v>
       </c>
       <c r="AE40" s="7" t="n">
-        <f aca="false">IF(Q40="TAK",Arkusz3!$B$24*J40,0)</f>
+        <f aca="false">IF(Q40="TAK",Arkusz3!$B$19*J40,0)</f>
         <v>5</v>
       </c>
       <c r="AF40" s="7" t="n">
-        <f aca="false">IF(R40="TAK",Arkusz3!$B$25*J40,0)</f>
-        <v>12</v>
+        <f aca="false">IF(R40="TAK",Arkusz3!$B$19*J40,0)</f>
+        <v>5</v>
       </c>
       <c r="AG40" s="7" t="n">
         <f aca="false">SUM(Z40:AF40)</f>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="AH40" s="7" t="n">
         <f aca="false">IF(L40="Nie",0,5)</f>
@@ -8085,7 +8073,7 @@
       </c>
       <c r="AP40" s="7" t="n">
         <f aca="false">IF(AI40&gt;5,AA40*0.2*(AI40-5)+AA40,AA40)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ40" s="7" t="n">
         <f aca="false">IF(AJ40&gt;5,AB40*0.2*(AJ40-5)+AB40,AB40)</f>
@@ -8105,15 +8093,15 @@
       </c>
       <c r="AU40" s="7" t="n">
         <f aca="false">IF(AN40&gt;5,AF40*0.2*(AN40-5)+AF40,AF40)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AV40" s="7" t="n">
         <f aca="false">SUM(AO40:AU40)+Y40</f>
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="AW40" s="7" t="n">
         <f aca="false">IF(S40="Roczna",AV40*12*0.95,AV40)</f>
-        <v>1162.8</v>
+        <v>1026</v>
       </c>
       <c r="AX40" s="7" t="s">
         <v>57</v>
@@ -8206,32 +8194,32 @@
         <v>0</v>
       </c>
       <c r="AA41" s="7" t="n">
-        <f aca="false">IF(M41="TAK",Arkusz3!$B$20*J41,0)</f>
-        <v>10</v>
+        <f aca="false">IF(M41="TAK",Arkusz3!$B$19*J41,0)</f>
+        <v>5</v>
       </c>
       <c r="AB41" s="7" t="n">
-        <f aca="false">IF(N41="TAK",Arkusz3!$B$21*J41,0)</f>
+        <f aca="false">IF(N41="TAK",Arkusz3!$B$19*J41,0)</f>
         <v>0</v>
       </c>
       <c r="AC41" s="7" t="n">
-        <f aca="false">IF(O41="TAK",Arkusz3!$B$22*J41,0)</f>
-        <v>10</v>
+        <f aca="false">IF(O41="TAK",Arkusz3!$B$19*J41,0)</f>
+        <v>5</v>
       </c>
       <c r="AD41" s="7" t="n">
-        <f aca="false">IF(P41="TAK",Arkusz3!$B$23*J41,0)</f>
+        <f aca="false">IF(P41="TAK",Arkusz3!$B$19*J41,0)</f>
         <v>0</v>
       </c>
       <c r="AE41" s="7" t="n">
-        <f aca="false">IF(Q41="TAK",Arkusz3!$B$24*J41,0)</f>
+        <f aca="false">IF(Q41="TAK",Arkusz3!$B$19*J41,0)</f>
         <v>5</v>
       </c>
       <c r="AF41" s="7" t="n">
-        <f aca="false">IF(R41="TAK",Arkusz3!$B$25*J41,0)</f>
+        <f aca="false">IF(R41="TAK",Arkusz3!$B$19*J41,0)</f>
         <v>0</v>
       </c>
       <c r="AG41" s="7" t="n">
         <f aca="false">SUM(Z41:AF41)</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AH41" s="7" t="n">
         <f aca="false">IF(L41="Nie",0,5)</f>
@@ -8265,7 +8253,7 @@
       </c>
       <c r="AP41" s="7" t="n">
         <f aca="false">IF(AI41&gt;5,AA41*0.2*(AI41-5)+AA41,AA41)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AQ41" s="7" t="n">
         <f aca="false">IF(AJ41&gt;5,AB41*0.2*(AJ41-5)+AB41,AB41)</f>
@@ -8273,7 +8261,7 @@
       </c>
       <c r="AR41" s="7" t="n">
         <f aca="false">IF(AK41&gt;5,AC41*0.2*(AK41-5)+AC41,AC41)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AS41" s="7" t="n">
         <f aca="false">IF(AL41&gt;5,AD41*0.2*(AL41-5)+AD41,AD41)</f>
@@ -8289,42 +8277,36 @@
       </c>
       <c r="AV41" s="7" t="n">
         <f aca="false">SUM(AO41:AU41)+Y41</f>
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="AW41" s="7" t="n">
         <f aca="false">IF(S41="Roczna",AV41*12*0.95,AV41)</f>
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="AX41" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="n">
-        <v>41</v>
-      </c>
-      <c r="D42" s="9" t="n">
-        <v>27</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="9" t="n">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K42" s="9" t="n">
+      <c r="K42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L42" s="1" t="s">
@@ -8334,7 +8316,7 @@
         <v>41</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>41</v>
@@ -8343,127 +8325,134 @@
         <v>41</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S42" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="S42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="T42" s="10" t="n">
+      <c r="T42" s="7" t="n">
         <f aca="false">G42*Arkusz3!$B$13+H42*Arkusz3!$B$14+I42*Arkusz3!$B$15</f>
         <v>0</v>
       </c>
-      <c r="U42" s="10" t="n">
+      <c r="U42" s="7" t="n">
         <f aca="false">IF((J42+F42)=1, Arkusz3!$C$5, Arkusz3!$B$5*J42)</f>
         <v>40</v>
       </c>
-      <c r="V42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="W42" s="10" t="n">
+      <c r="V42" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="W42" s="7" t="n">
         <f aca="false">IF(V42&lt;10,T42+U42,0.2*(V42-10)*(T42+U42)+(T42+U42))</f>
         <v>40</v>
       </c>
-      <c r="X42" s="10" t="n">
+      <c r="X42" s="7" t="n">
         <f aca="false">IF(J42&gt;1,(U42/J42)*(J42-1)*10%,0)</f>
         <v>0</v>
       </c>
-      <c r="Y42" s="11" t="n">
+      <c r="Y42" s="8" t="n">
         <f aca="false">W42-X42</f>
         <v>40</v>
       </c>
-      <c r="Z42" s="10" t="n">
+      <c r="Z42" s="7" t="n">
         <f aca="false">IF(L42="TAK",Arkusz3!$B$19*J42,0)</f>
         <v>0</v>
       </c>
-      <c r="AA42" s="10" t="n">
-        <f aca="false">IF(M42="TAK",Arkusz3!$B$20*J42,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB42" s="10" t="n">
-        <f aca="false">IF(N42="TAK",Arkusz3!$B$21*J42,0)</f>
-        <v>8</v>
-      </c>
-      <c r="AC42" s="10" t="n">
-        <f aca="false">IF(O42="TAK",Arkusz3!$B$22*J42,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD42" s="10" t="n">
-        <f aca="false">IF(P42="TAK",Arkusz3!$B$23*J42,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE42" s="10" t="n">
-        <f aca="false">IF(Q42="TAK",Arkusz3!$B$24*J42,0)</f>
-        <v>5</v>
-      </c>
-      <c r="AF42" s="10" t="n">
-        <f aca="false">IF(R42="TAK",Arkusz3!$B$25*J42,0)</f>
-        <v>12</v>
-      </c>
-      <c r="AG42" s="10" t="n">
+      <c r="AA42" s="7" t="n">
+        <f aca="false">IF(M42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="7" t="n">
+        <f aca="false">IF(N42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC42" s="7" t="n">
+        <f aca="false">IF(O42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="7" t="n">
+        <f aca="false">IF(P42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE42" s="7" t="n">
+        <f aca="false">IF(Q42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF42" s="7" t="n">
+        <f aca="false">IF(R42="TAK",Arkusz3!$B$19*J42,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG42" s="7" t="n">
         <f aca="false">SUM(Z42:AF42)</f>
-        <v>25</v>
-      </c>
-      <c r="AH42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AK42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AL42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AM42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AN42" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AO42" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="7" t="n">
+        <f aca="false">IF(L42="Nie",0,5)</f>
+        <v>0</v>
+      </c>
+      <c r="AI42" s="7" t="n">
+        <f aca="false">IF(M42="Nie",0,5)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="7" t="n">
+        <f aca="false">IF(N42="Nie",0,5)</f>
+        <v>0</v>
+      </c>
+      <c r="AK42" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="7" t="n">
+        <f aca="false">IF(P42="Nie",0,5)</f>
+        <v>0</v>
+      </c>
+      <c r="AM42" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN42" s="7" t="n">
+        <f aca="false">IF(R42="Nie",0,5)</f>
+        <v>0</v>
+      </c>
+      <c r="AO42" s="7" t="n">
         <f aca="false">IF(AH42&gt;5,Z42*0.2*(AH42-5)+Z42,Z42)</f>
         <v>0</v>
       </c>
-      <c r="AP42" s="10" t="n">
+      <c r="AP42" s="7" t="n">
         <f aca="false">IF(AI42&gt;5,AA42*0.2*(AI42-5)+AA42,AA42)</f>
         <v>0</v>
       </c>
-      <c r="AQ42" s="10" t="n">
+      <c r="AQ42" s="7" t="n">
         <f aca="false">IF(AJ42&gt;5,AB42*0.2*(AJ42-5)+AB42,AB42)</f>
-        <v>16</v>
-      </c>
-      <c r="AR42" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR42" s="7" t="n">
         <f aca="false">IF(AK42&gt;5,AC42*0.2*(AK42-5)+AC42,AC42)</f>
         <v>0</v>
       </c>
-      <c r="AS42" s="10" t="n">
+      <c r="AS42" s="7" t="n">
         <f aca="false">IF(AL42&gt;5,AD42*0.2*(AL42-5)+AD42,AD42)</f>
         <v>0</v>
       </c>
-      <c r="AT42" s="10" t="n">
+      <c r="AT42" s="7" t="n">
         <f aca="false">IF(AM42&gt;5,AE42*0.2*(AM42-5)+AE42,AE42)</f>
-        <v>10</v>
-      </c>
-      <c r="AU42" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU42" s="7" t="n">
         <f aca="false">IF(AN42&gt;5,AF42*0.2*(AN42-5)+AF42,AF42)</f>
-        <v>24</v>
-      </c>
-      <c r="AV42" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV42" s="7" t="n">
         <f aca="false">SUM(AO42:AU42)+Y42</f>
-        <v>90</v>
-      </c>
-      <c r="AW42" s="10" t="n">
+        <v>40</v>
+      </c>
+      <c r="AW42" s="7" t="n">
         <f aca="false">IF(S42="Roczna",AV42*12*0.95,AV42)</f>
-        <v>1026</v>
-      </c>
-      <c r="AX42" s="10"/>
+        <v>456</v>
+      </c>
+      <c r="AX42" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -9455,15 +9444,15 @@
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17"/>
@@ -9472,68 +9461,68 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="13" t="n">
+      <c r="B1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="10" t="n">
         <v>0.1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="13" t="n">
+      <c r="F1" s="10" t="n">
         <v>0.05</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="14" t="n">
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11" t="n">
         <v>0.2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="G4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="13" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="7" t="n">
@@ -9559,7 +9548,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="G6" s="7" t="s">
@@ -9579,7 +9568,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="G7" s="7" t="s">
@@ -9599,7 +9588,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B8" s="7" t="n">
@@ -9610,114 +9599,114 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="19" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="24" t="n">
+      <c r="B14" s="21" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="19" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C19" s="12"/>
+      <c r="B19" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="9"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="C20" s="12"/>
+      <c r="B20" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="12" t="n">
+      <c r="B21" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="B22" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="12" t="n">
+      <c r="B23" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="12" t="n">
+      <c r="B25" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10726,97 +10715,97 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="18" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="25" t="s">
+      <c r="J1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="T1" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="U1" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="W1" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="Y1" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AA1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="22" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10899,7 +10888,7 @@
       <c r="Z2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="26" t="n">
+      <c r="AA2" s="23" t="n">
         <v>404.5</v>
       </c>
       <c r="AB2" s="7" t="s">
@@ -10985,7 +10974,7 @@
       <c r="Z3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA3" s="26" t="n">
+      <c r="AA3" s="23" t="n">
         <v>3539.7</v>
       </c>
       <c r="AB3" s="7" t="s">
@@ -11071,7 +11060,7 @@
       <c r="Z4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="26" t="n">
+      <c r="AA4" s="23" t="n">
         <v>1197</v>
       </c>
       <c r="AB4" s="7" t="s">
@@ -11157,7 +11146,7 @@
       <c r="Z5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA5" s="26" t="n">
+      <c r="AA5" s="23" t="n">
         <v>264.5</v>
       </c>
       <c r="AB5" s="7" t="s">
@@ -11243,7 +11232,7 @@
       <c r="Z6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA6" s="26" t="n">
+      <c r="AA6" s="23" t="n">
         <v>169</v>
       </c>
       <c r="AB6" s="7" t="s">
@@ -11329,7 +11318,7 @@
       <c r="Z7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="26" t="n">
+      <c r="AA7" s="23" t="n">
         <v>264.5</v>
       </c>
       <c r="AB7" s="7" t="s">
@@ -11415,7 +11404,7 @@
       <c r="Z8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA8" s="26" t="n">
+      <c r="AA8" s="23" t="n">
         <v>175</v>
       </c>
       <c r="AB8" s="7" t="s">
@@ -11501,7 +11490,7 @@
       <c r="Z9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA9" s="26" t="n">
+      <c r="AA9" s="23" t="n">
         <v>200</v>
       </c>
       <c r="AB9" s="7" t="s">
@@ -11587,7 +11576,7 @@
       <c r="Z10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA10" s="26" t="n">
+      <c r="AA10" s="23" t="n">
         <v>95</v>
       </c>
       <c r="AB10" s="7" t="s">
@@ -11673,7 +11662,7 @@
       <c r="Z11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA11" s="26" t="n">
+      <c r="AA11" s="23" t="n">
         <v>95</v>
       </c>
       <c r="AB11" s="7" t="s">
@@ -11759,7 +11748,7 @@
       <c r="Z12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA12" s="26" t="n">
+      <c r="AA12" s="23" t="n">
         <v>284.5</v>
       </c>
       <c r="AB12" s="7" t="s">
@@ -11845,7 +11834,7 @@
       <c r="Z13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA13" s="26" t="n">
+      <c r="AA13" s="23" t="n">
         <v>244.5</v>
       </c>
       <c r="AB13" s="7" t="s">
@@ -11931,7 +11920,7 @@
       <c r="Z14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA14" s="26" t="n">
+      <c r="AA14" s="23" t="n">
         <v>1083</v>
       </c>
       <c r="AB14" s="7" t="s">
@@ -12017,7 +12006,7 @@
       <c r="Z15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA15" s="26" t="n">
+      <c r="AA15" s="23" t="n">
         <v>496.5</v>
       </c>
       <c r="AB15" s="7" t="s">
@@ -12103,7 +12092,7 @@
       <c r="Z16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA16" s="26" t="n">
+      <c r="AA16" s="23" t="n">
         <v>110</v>
       </c>
       <c r="AB16" s="7" t="s">
@@ -12189,7 +12178,7 @@
       <c r="Z17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA17" s="26" t="n">
+      <c r="AA17" s="23" t="n">
         <v>160</v>
       </c>
       <c r="AB17" s="7" t="s">
@@ -12275,7 +12264,7 @@
       <c r="Z18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA18" s="26" t="n">
+      <c r="AA18" s="23" t="n">
         <v>3608.1</v>
       </c>
       <c r="AB18" s="7" t="s">
@@ -12361,7 +12350,7 @@
       <c r="Z19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA19" s="26" t="n">
+      <c r="AA19" s="23" t="n">
         <v>2946.9</v>
       </c>
       <c r="AB19" s="7" t="s">
@@ -12447,7 +12436,7 @@
       <c r="Z20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA20" s="26" t="n">
+      <c r="AA20" s="23" t="n">
         <v>374.5</v>
       </c>
       <c r="AB20" s="7" t="s">
@@ -12533,7 +12522,7 @@
       <c r="Z21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA21" s="26" t="n">
+      <c r="AA21" s="23" t="n">
         <v>111</v>
       </c>
       <c r="AB21" s="7" t="s">
@@ -12619,7 +12608,7 @@
       <c r="Z22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA22" s="26" t="n">
+      <c r="AA22" s="23" t="n">
         <v>264.5</v>
       </c>
       <c r="AB22" s="7" t="s">
@@ -12705,7 +12694,7 @@
       <c r="Z23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA23" s="26" t="n">
+      <c r="AA23" s="23" t="n">
         <v>335</v>
       </c>
       <c r="AB23" s="7" t="s">
@@ -12791,7 +12780,7 @@
       <c r="Z24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA24" s="26" t="n">
+      <c r="AA24" s="23" t="n">
         <v>170</v>
       </c>
       <c r="AB24" s="7" t="s">
@@ -12877,7 +12866,7 @@
       <c r="Z25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA25" s="26" t="n">
+      <c r="AA25" s="23" t="n">
         <v>150</v>
       </c>
       <c r="AB25" s="7" t="s">
@@ -12963,7 +12952,7 @@
       <c r="Z26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA26" s="26" t="n">
+      <c r="AA26" s="23" t="n">
         <v>170.5</v>
       </c>
       <c r="AB26" s="7" t="s">
@@ -13049,7 +13038,7 @@
       <c r="Z27" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA27" s="26" t="n">
+      <c r="AA27" s="23" t="n">
         <v>374.5</v>
       </c>
       <c r="AB27" s="7" t="s">
@@ -13135,7 +13124,7 @@
       <c r="Z28" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA28" s="26" t="n">
+      <c r="AA28" s="23" t="n">
         <v>135</v>
       </c>
       <c r="AB28" s="7" t="s">
@@ -13221,7 +13210,7 @@
       <c r="Z29" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA29" s="26" t="n">
+      <c r="AA29" s="23" t="n">
         <v>145</v>
       </c>
       <c r="AB29" s="7" t="s">
@@ -13307,7 +13296,7 @@
       <c r="Z30" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA30" s="26" t="n">
+      <c r="AA30" s="23" t="n">
         <v>534.5</v>
       </c>
       <c r="AB30" s="7" t="s">
@@ -13393,7 +13382,7 @@
       <c r="Z31" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA31" s="26" t="n">
+      <c r="AA31" s="23" t="n">
         <v>86</v>
       </c>
       <c r="AB31" s="7" t="s">
@@ -13479,7 +13468,7 @@
       <c r="Z32" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA32" s="26" t="n">
+      <c r="AA32" s="23" t="n">
         <v>190</v>
       </c>
       <c r="AB32" s="7" t="s">
@@ -13565,7 +13554,7 @@
       <c r="Z33" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA33" s="26" t="n">
+      <c r="AA33" s="23" t="n">
         <v>304.5</v>
       </c>
       <c r="AB33" s="7" t="s">
@@ -13651,7 +13640,7 @@
       <c r="Z34" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA34" s="26" t="n">
+      <c r="AA34" s="23" t="n">
         <v>55</v>
       </c>
       <c r="AB34" s="7" t="s">
@@ -13737,7 +13726,7 @@
       <c r="Z35" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA35" s="26" t="n">
+      <c r="AA35" s="23" t="n">
         <v>215</v>
       </c>
       <c r="AB35" s="7" t="s">
@@ -13823,7 +13812,7 @@
       <c r="Z36" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA36" s="26" t="n">
+      <c r="AA36" s="23" t="n">
         <v>4611.3</v>
       </c>
       <c r="AB36" s="7" t="s">
@@ -13909,7 +13898,7 @@
       <c r="Z37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA37" s="26" t="n">
+      <c r="AA37" s="23" t="n">
         <v>410.4</v>
       </c>
       <c r="AB37" s="7" t="s">
@@ -13995,7 +13984,7 @@
       <c r="Z38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA38" s="26" t="n">
+      <c r="AA38" s="23" t="n">
         <v>1995</v>
       </c>
       <c r="AB38" s="7" t="s">
@@ -14081,7 +14070,7 @@
       <c r="Z39" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA39" s="26" t="n">
+      <c r="AA39" s="23" t="n">
         <v>324.5</v>
       </c>
       <c r="AB39" s="7" t="s">
@@ -14167,7 +14156,7 @@
       <c r="Z40" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA40" s="26" t="n">
+      <c r="AA40" s="23" t="n">
         <v>1539</v>
       </c>
       <c r="AB40" s="7" t="s">
@@ -14253,7 +14242,7 @@
       <c r="Z41" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA41" s="26" t="n">
+      <c r="AA41" s="23" t="n">
         <v>105</v>
       </c>
       <c r="AB41" s="7" t="s">

</xml_diff>